<commit_message>
final cleanup + readme
</commit_message>
<xml_diff>
--- a/Addition_Unit/Documentation/ProjectLog-G12-4255-350-1257.xlsx
+++ b/Addition_Unit/Documentation/ProjectLog-G12-4255-350-1257.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CACE8BEB-024A-4653-AA14-6813A45756F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F2C9372-8804-4F14-878C-6FED346C44F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="uphip+fyQmgTbQWVslgKndYGTCUT2nMCnU8pTyuiPxh9t3MkaNQeLeeV1eDZUH8uYM8JtsIZJzZApwnnbRUEcA==" workbookSaltValue="PVE5+bPUyqyV9jE5EaqSxw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3276" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5C666647-60C4-4C14-A5E1-8900F85EBB7F}"/>
   </bookViews>
   <sheets>
     <sheet name="DP1.0" sheetId="5" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
   <si>
     <t>last  4 digits</t>
   </si>
@@ -453,7 +453,46 @@
     <t>read over other sections of the report made multiple edits</t>
   </si>
   <si>
-    <t>final read over and minor edits</t>
+    <t>minor edits</t>
+  </si>
+  <si>
+    <t>redid cost calculations using analygous boards for a more accurate LE to ALM conversion</t>
+  </si>
+  <si>
+    <t>anotating images and editing</t>
+  </si>
+  <si>
+    <t>implemented a carry look ahead tree architecture for the adder</t>
+  </si>
+  <si>
+    <t>finished brent kung adder</t>
+  </si>
+  <si>
+    <t>got all candidates quartus summaries and .vho and .sdo files</t>
+  </si>
+  <si>
+    <t>wrote and debugged a 4 bit look ahead carry network component</t>
+  </si>
+  <si>
+    <t>worked on the report specifically the the testbench section</t>
+  </si>
+  <si>
+    <t>Figured out timing simulations</t>
+  </si>
+  <si>
+    <t>worked on the test bench to prepare it for timing simulations</t>
+  </si>
+  <si>
+    <t>worked on the testbench and helped write .do files</t>
+  </si>
+  <si>
+    <t>wrote last candidate the carry-bypass adder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worked on the report edits and images. </t>
+  </si>
+  <si>
+    <t>worked on the summary</t>
   </si>
 </sst>
 </file>
@@ -902,7 +941,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1081,6 +1120,42 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -5146,8 +5221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFECA045-CD49-49CC-91F4-D8E7747F6F1D}">
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5323,28 +5398,48 @@
     </row>
     <row r="10" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
+      <c r="B10" s="13">
+        <v>4255</v>
+      </c>
+      <c r="C10" s="21">
+        <v>45955</v>
+      </c>
+      <c r="D10" s="19">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E10" s="22">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="16" t="s">
+        <v>34</v>
+      </c>
       <c r="H10" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.4999999999999982</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="B11" s="13">
+        <v>4255</v>
+      </c>
+      <c r="C11" s="21">
+        <v>45956</v>
+      </c>
+      <c r="D11" s="19">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E11" s="22">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="16"/>
+      <c r="G11" s="16" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9999999999999982</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -6235,7 +6330,7 @@
       <c r="F80" s="29"/>
       <c r="H80" s="28">
         <f>SUM(H7:H79)</f>
-        <v>3</v>
+        <v>8.4999999999999964</v>
       </c>
     </row>
     <row r="81" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -6966,7 +7061,7 @@
   <dimension ref="A1:I783"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6998,7 +7093,9 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="50" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -7011,7 +7108,9 @@
       <c r="A3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="53">
+        <v>301454255</v>
+      </c>
       <c r="C3" s="54"/>
       <c r="D3" s="55"/>
       <c r="E3" s="46"/>
@@ -8754,8 +8853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAC5635-BB81-4716-B442-28EF74567593}">
   <dimension ref="A1:I783"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8787,7 +8886,9 @@
       <c r="A2" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
+      <c r="B2" s="50" t="s">
+        <v>20</v>
+      </c>
       <c r="C2" s="51"/>
       <c r="D2" s="52"/>
       <c r="E2" s="44" t="s">
@@ -8800,7 +8901,9 @@
       <c r="A3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="53"/>
+      <c r="B3" s="53">
+        <v>301454255</v>
+      </c>
       <c r="C3" s="54"/>
       <c r="D3" s="55"/>
       <c r="E3" s="46"/>
@@ -8824,8 +8927,8 @@
       <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="56" t="s">
-        <v>12</v>
+      <c r="B5" s="41">
+        <v>0.45</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="43"/>
@@ -8861,146 +8964,256 @@
     </row>
     <row r="7" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
+      <c r="B7" s="57">
+        <v>4255</v>
+      </c>
+      <c r="C7" s="59">
+        <v>45960</v>
+      </c>
+      <c r="D7" s="60">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E7" s="61">
+        <v>0.8125</v>
+      </c>
       <c r="F7" s="33"/>
-      <c r="G7" s="15"/>
+      <c r="G7" s="64" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" s="11">
         <f t="shared" ref="H7" si="0">(E7-D7)*24</f>
-        <v>0</v>
+        <v>2.4999999999999991</v>
       </c>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="31"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="22"/>
+      <c r="B8" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C8" s="62">
+        <v>45961</v>
+      </c>
+      <c r="D8" s="60">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E8" s="63">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F8" s="34"/>
-      <c r="G8" s="16"/>
+      <c r="G8" s="65" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="26">
         <f>(E8-D8)*24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="31"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="22"/>
+      <c r="B9" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C9" s="62">
+        <v>45965</v>
+      </c>
+      <c r="D9" s="60">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E9" s="63">
+        <v>0.8125</v>
+      </c>
       <c r="F9" s="34"/>
-      <c r="G9" s="16"/>
+      <c r="G9" s="65" t="s">
+        <v>37</v>
+      </c>
       <c r="H9" s="26">
         <f t="shared" ref="H9:H72" si="1">(E9-D9)*24</f>
-        <v>0</v>
+        <v>3.5000000000000009</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="22"/>
+      <c r="B10" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C10" s="62">
+        <v>45972</v>
+      </c>
+      <c r="D10" s="60">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E10" s="63">
+        <v>0.75</v>
+      </c>
       <c r="F10" s="34"/>
-      <c r="G10" s="16"/>
+      <c r="G10" s="65" t="s">
+        <v>41</v>
+      </c>
       <c r="H10" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="31"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="22"/>
+      <c r="B11" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C11" s="62">
+        <v>45973</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0.625</v>
+      </c>
+      <c r="E11" s="63">
+        <v>0.6875</v>
+      </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="16"/>
+      <c r="G11" s="65" t="s">
+        <v>42</v>
+      </c>
       <c r="H11" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="31"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="22"/>
+      <c r="B12" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C12" s="62">
+        <v>45973</v>
+      </c>
+      <c r="D12" s="60">
+        <v>0.6875</v>
+      </c>
+      <c r="E12" s="63">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F12" s="34"/>
-      <c r="G12" s="16"/>
+      <c r="G12" s="65" t="s">
+        <v>38</v>
+      </c>
       <c r="H12" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="31"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="22"/>
+      <c r="B13" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C13" s="62">
+        <v>45973</v>
+      </c>
+      <c r="D13" s="60">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E13" s="63">
+        <v>0.8125</v>
+      </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="16"/>
+      <c r="G13" s="65" t="s">
+        <v>43</v>
+      </c>
       <c r="H13" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="31"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="22"/>
+      <c r="B14" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C14" s="62">
+        <v>45974</v>
+      </c>
+      <c r="D14" s="60">
+        <v>0.625</v>
+      </c>
+      <c r="E14" s="63">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F14" s="34"/>
-      <c r="G14" s="16"/>
+      <c r="G14" s="65" t="s">
+        <v>44</v>
+      </c>
       <c r="H14" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.9999999999999991</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="31"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="22"/>
+      <c r="B15" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C15" s="62">
+        <v>45976</v>
+      </c>
+      <c r="D15" s="60">
+        <v>0.75</v>
+      </c>
+      <c r="E15" s="63">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="F15" s="34"/>
-      <c r="G15" s="16"/>
+      <c r="G15" s="65" t="s">
+        <v>40</v>
+      </c>
       <c r="H15" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="31"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
+      <c r="B16" s="58">
+        <v>4255</v>
+      </c>
+      <c r="C16" s="62">
+        <v>45977</v>
+      </c>
+      <c r="D16" s="60">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E16" s="63">
+        <v>0.83333333333333337</v>
+      </c>
       <c r="F16" s="34"/>
-      <c r="G16" s="16"/>
+      <c r="G16" s="65" t="s">
+        <v>45</v>
+      </c>
       <c r="H16" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.5000000000000018</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="31"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="22"/>
+      <c r="B17" s="13">
+        <v>4255</v>
+      </c>
+      <c r="C17" s="21">
+        <v>45977</v>
+      </c>
+      <c r="D17" s="19">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E17" s="22">
+        <v>0.875</v>
+      </c>
       <c r="F17" s="34"/>
-      <c r="G17" s="16"/>
+      <c r="G17" s="16" t="s">
+        <v>46</v>
+      </c>
       <c r="H17" s="26">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="24.9" customHeight="1" x14ac:dyDescent="0.35">
@@ -9813,7 +10026,7 @@
       <c r="F80" s="29"/>
       <c r="H80" s="28">
         <f>SUM(H7:H79)</f>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="81" ht="24.9" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>